<commit_message>
updates in language learning pom
</commit_message>
<xml_diff>
--- a/testData/Output.xlsx
+++ b/testData/Output.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="98">
   <si>
     <t>Meta Front-End Developer</t>
   </si>
@@ -258,6 +258,69 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>English (1,625)</t>
+  </si>
+  <si>
+    <t>Mixed(124)</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Portuguese (Brazil) (949)</t>
+  </si>
+  <si>
+    <t>Mixed(120)</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Arabic (974)</t>
+  </si>
+  <si>
+    <t>French (958)</t>
+  </si>
+  <si>
+    <t>Spanish (1,062)</t>
+  </si>
+  <si>
+    <t>Mixed(131)</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>733</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>819</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>583</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>907</t>
+  </si>
+  <si>
+    <t>754</t>
+  </si>
+  <si>
+    <t>452</t>
+  </si>
+  <si>
+    <t>537</t>
   </si>
 </sst>
 </file>
@@ -606,10 +669,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -617,10 +680,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -686,7 +749,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -708,7 +771,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -716,7 +779,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -732,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -754,7 +817,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -762,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -770,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -778,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -794,13 +857,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -808,53 +871,53 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -862,15 +925,15 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>